<commit_message>
Add New Parking Function
</commit_message>
<xml_diff>
--- a/CarFile.xlsx
+++ b/CarFile.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2hgt131</t>
+          <t>2hgt132</t>
         </is>
       </c>
     </row>
@@ -582,41 +582,41 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2hgt132</t>
+          <t>2hgt133</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>vw</t>
+          <t>fiat</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>golf</t>
+          <t>500</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2hgt133</t>
+          <t>1SSS333</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>fiat</t>
+          <t>vw</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>golf</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1SSS333</t>
+          <t>2hgt135</t>
         </is>
       </c>
     </row>
@@ -633,56 +633,39 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2hgt135</t>
+          <t>2hgt136</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>vw</t>
+          <t>mercedes</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>golf</t>
+          <t>c180</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2hgt136</t>
+          <t>1vgg250</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>mercedes</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>c180</t>
+          <t>v40</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
-        <is>
-          <t>1vgg250</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>v40</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
         <is>
           <t>1fgt362</t>
         </is>

</xml_diff>